<commit_message>
Debuging incorrect values on output
Expand distance bus and add debug hooks.
</commit_message>
<xml_diff>
--- a/Docs/test1.xlsx
+++ b/Docs/test1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="14370"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="14370" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,6 +34,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -63,11 +66,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -371,7 +375,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
@@ -581,13 +585,141 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="20.7109375" customWidth="1"/>
+    <col min="3" max="3" width="28" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>17</v>
+      </c>
+      <c r="B1" s="2">
+        <v>2378858632.4404702</v>
+      </c>
+      <c r="C1">
+        <f>POWER(B1,2)</f>
+        <v>5.6589683931365437E+18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>13</v>
+      </c>
+      <c r="B2" s="2">
+        <v>2546340798.0274501</v>
+      </c>
+      <c r="C2">
+        <f t="shared" ref="C2:C9" si="0">POWER(B2,2)</f>
+        <v>6.483851459699071E+18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>10</v>
+      </c>
+      <c r="B3" s="2">
+        <v>2671753018.757</v>
+      </c>
+      <c r="C3">
+        <f t="shared" si="0"/>
+        <v>7.1382641932371425E+18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>11</v>
+      </c>
+      <c r="B4" s="2">
+        <v>2894561484.2773299</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>8.3784861862617795E+18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>48</v>
+      </c>
+      <c r="B5" s="2">
+        <v>2918228302.5657401</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>8.516056425895721E+18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>26</v>
+      </c>
+      <c r="B6" s="2">
+        <v>3089562004.6875601</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>9.5453933808090153E+18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>60</v>
+      </c>
+      <c r="B7" s="2">
+        <v>3090682997.1241899</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>9.5523213887125647E+18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>56</v>
+      </c>
+      <c r="B8" s="2">
+        <v>3109507391.0303402</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>9.6690362148723139E+18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>62</v>
+      </c>
+      <c r="B9" s="2">
+        <v>3123623195.41642</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>9.757021866943486E+18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>16</v>
+      </c>
+      <c r="B10" s="2">
+        <v>3125181049.6946502</v>
+      </c>
+      <c r="C10">
+        <f>POWER(B10,2)</f>
+        <v>9.7667565933705564E+18</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Debugging incorrect result output
final results are wrong when readout
</commit_message>
<xml_diff>
--- a/Docs/test1.xlsx
+++ b/Docs/test1.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="14370" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="14370" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" fullPrecision="0"/>
 </workbook>
 </file>
 
@@ -66,12 +66,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -426,7 +429,7 @@
       </c>
       <c r="H2">
         <f>SQRT(G2)</f>
-        <v>12.767145334803704</v>
+        <v>12.767145334803701</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -454,7 +457,7 @@
       </c>
       <c r="H3">
         <f>SQRT(G3)</f>
-        <v>2.6457513110645907</v>
+        <v>2.6457513110645898</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -482,7 +485,7 @@
       </c>
       <c r="H4">
         <f t="shared" ref="H4:H6" si="0">SQRT(G4)</f>
-        <v>1.4142135623730951</v>
+        <v>1.4142135623731</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -510,7 +513,7 @@
       </c>
       <c r="H5">
         <f t="shared" si="0"/>
-        <v>1.4142135623730951</v>
+        <v>1.4142135623731</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -538,7 +541,7 @@
       </c>
       <c r="H6">
         <f t="shared" si="0"/>
-        <v>6.8556546004010439</v>
+        <v>6.8556546004010404</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -587,8 +590,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -606,7 +609,7 @@
       </c>
       <c r="C1">
         <f>POWER(B1,2)</f>
-        <v>5.6589683931365437E+18</v>
+        <v>5.6589683931365396E+18</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -618,7 +621,7 @@
       </c>
       <c r="C2">
         <f t="shared" ref="C2:C9" si="0">POWER(B2,2)</f>
-        <v>6.483851459699071E+18</v>
+        <v>6.48385145969907E+18</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -630,7 +633,7 @@
       </c>
       <c r="C3">
         <f t="shared" si="0"/>
-        <v>7.1382641932371425E+18</v>
+        <v>7.1382641932371405E+18</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -642,7 +645,7 @@
       </c>
       <c r="C4">
         <f t="shared" si="0"/>
-        <v>8.3784861862617795E+18</v>
+        <v>8.3784861862617805E+18</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -654,7 +657,7 @@
       </c>
       <c r="C5">
         <f t="shared" si="0"/>
-        <v>8.516056425895721E+18</v>
+        <v>8.5160564258957199E+18</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -666,7 +669,7 @@
       </c>
       <c r="C6">
         <f t="shared" si="0"/>
-        <v>9.5453933808090153E+18</v>
+        <v>9.5453933808090194E+18</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -678,7 +681,7 @@
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>9.5523213887125647E+18</v>
+        <v>9.5523213887125606E+18</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -690,7 +693,7 @@
       </c>
       <c r="C8">
         <f t="shared" si="0"/>
-        <v>9.6690362148723139E+18</v>
+        <v>9.6690362148723098E+18</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -702,7 +705,7 @@
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>9.757021866943486E+18</v>
+        <v>9.75702186694349E+18</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -714,7 +717,7 @@
       </c>
       <c r="C10">
         <f>POWER(B10,2)</f>
-        <v>9.7667565933705564E+18</v>
+        <v>9.7667565933705605E+18</v>
       </c>
     </row>
   </sheetData>
@@ -725,12 +728,300 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="22" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <v>2</v>
+      </c>
+      <c r="C1">
+        <v>2</v>
+      </c>
+      <c r="D1">
+        <v>2</v>
+      </c>
+      <c r="E1">
+        <v>3</v>
+      </c>
+      <c r="F1">
+        <v>4</v>
+      </c>
+      <c r="G1">
+        <v>5</v>
+      </c>
+      <c r="H1">
+        <v>5</v>
+      </c>
+      <c r="I1">
+        <v>5</v>
+      </c>
+      <c r="J1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>587346851</v>
+      </c>
+      <c r="B2">
+        <v>1375896618</v>
+      </c>
+      <c r="C2">
+        <v>1091532660</v>
+      </c>
+      <c r="D2">
+        <v>1049174902</v>
+      </c>
+      <c r="E2">
+        <v>572047254</v>
+      </c>
+      <c r="F2">
+        <v>385621721</v>
+      </c>
+      <c r="G2">
+        <v>1657189250</v>
+      </c>
+      <c r="H2">
+        <v>213706809</v>
+      </c>
+      <c r="I2">
+        <v>585249083</v>
+      </c>
+      <c r="J2">
+        <v>1962287530</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <f>A1-A2</f>
+        <v>-587346850</v>
+      </c>
+      <c r="B3">
+        <f>B1-B2</f>
+        <v>-1375896616</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:J3" si="0">C1-C2</f>
+        <v>-1091532658</v>
+      </c>
+      <c r="D3">
+        <f t="shared" si="0"/>
+        <v>-1049174900</v>
+      </c>
+      <c r="E3">
+        <f t="shared" si="0"/>
+        <v>-572047251</v>
+      </c>
+      <c r="F3">
+        <f t="shared" si="0"/>
+        <v>-385621717</v>
+      </c>
+      <c r="G3">
+        <f t="shared" si="0"/>
+        <v>-1657189245</v>
+      </c>
+      <c r="H3">
+        <f t="shared" si="0"/>
+        <v>-213706804</v>
+      </c>
+      <c r="I3">
+        <f t="shared" si="0"/>
+        <v>-585249078</v>
+      </c>
+      <c r="J3">
+        <f t="shared" si="0"/>
+        <v>-1962287524</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <f>A3*A3</f>
+        <v>3.4497632220492198E+17</v>
+      </c>
+      <c r="B4" s="5">
+        <f>POWER(B3, 2)</f>
+        <v>1.8930914979202501E+18</v>
+      </c>
+      <c r="C4" s="3">
+        <f t="shared" ref="C4:J4" si="1">POWER(C3, 2)</f>
+        <v>1.1914435434805499E+18</v>
+      </c>
+      <c r="D4" s="3">
+        <f t="shared" si="1"/>
+        <v>1.10076797079001E+18</v>
+      </c>
+      <c r="E4" s="3">
+        <f t="shared" si="1"/>
+        <v>3.2723805737665702E+17</v>
+      </c>
+      <c r="F4" s="3">
+        <f t="shared" si="1"/>
+        <v>1.48704108622028E+17</v>
+      </c>
+      <c r="G4" s="3">
+        <f t="shared" si="1"/>
+        <v>2.7462761937436698E+18</v>
+      </c>
+      <c r="H4" s="3">
+        <f t="shared" si="1"/>
+        <v>4.56705980758944E+16</v>
+      </c>
+      <c r="I4" s="3">
+        <f t="shared" si="1"/>
+        <v>3.4251648329984998E+17</v>
+      </c>
+      <c r="J4" s="3">
+        <f t="shared" si="1"/>
+        <v>3.8505723268460498E+18</v>
+      </c>
+      <c r="K4" s="4">
+        <f>SUM(A4:J4)</f>
+        <v>1.19912571023599E+19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>10</v>
+      </c>
+      <c r="B7" s="3">
+        <v>2671753018.757</v>
+      </c>
+      <c r="C7" s="3">
+        <f>POWER(B7,2)</f>
+        <v>7.1382641932371405E+18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>9</v>
+      </c>
+      <c r="B8" s="3">
+        <v>3252129437.44803</v>
+      </c>
+      <c r="C8" s="3">
+        <f t="shared" ref="C8:C16" si="2">POWER(B8,2)</f>
+        <v>1.0576345877916E+19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>3</v>
+      </c>
+      <c r="B9" s="3">
+        <v>3424195240.61727</v>
+      </c>
+      <c r="C9" s="3">
+        <f t="shared" si="2"/>
+        <v>1.1725113045866E+19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>0</v>
+      </c>
+      <c r="B10" s="3">
+        <v>3462839456.6251302</v>
+      </c>
+      <c r="C10" s="3">
+        <f t="shared" si="2"/>
+        <v>1.19912571023598E+19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11" s="3">
+        <v>3577151753.3151498</v>
+      </c>
+      <c r="C11" s="3">
+        <f t="shared" si="2"/>
+        <v>1.27960146662457E+19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>8</v>
+      </c>
+      <c r="B12" s="3">
+        <v>3746510094.0608602</v>
+      </c>
+      <c r="C12" s="3">
+        <f t="shared" si="2"/>
+        <v>1.4036337884899899E+19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>6</v>
+      </c>
+      <c r="B13" s="3">
+        <v>3941785051.40452</v>
+      </c>
+      <c r="C13" s="3">
+        <f t="shared" si="2"/>
+        <v>1.5537669391476099E+19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>7</v>
+      </c>
+      <c r="B14" s="3">
+        <v>4107660439.7937598</v>
+      </c>
+      <c r="C14" s="3">
+        <f t="shared" si="2"/>
+        <v>1.6872874288646699E+19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>5</v>
+      </c>
+      <c r="B15" s="3">
+        <v>4325266764.1720896</v>
+      </c>
+      <c r="C15" s="3">
+        <f t="shared" si="2"/>
+        <v>1.8707932581251699E+19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>4</v>
+      </c>
+      <c r="B16" s="3">
+        <v>4401994956.3000002</v>
+      </c>
+      <c r="C16" s="3">
+        <f t="shared" si="2"/>
+        <v>1.9377559595290599E+19</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Large data set working
10000 points
</commit_message>
<xml_diff>
--- a/Docs/test1.xlsx
+++ b/Docs/test1.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dakota\Documents\Github\Thesis\Docs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="14370" activeTab="2"/>
   </bookViews>
@@ -11,12 +16,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621" fullPrecision="0"/>
+  <calcPr calcId="152511" fullPrecision="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>ref</t>
   </si>
@@ -29,13 +34,20 @@
   <si>
     <t>k=3</t>
   </si>
+  <si>
+    <t>10000 data set</t>
+  </si>
+  <si>
+    <t>answers</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000000"/>
+    <numFmt numFmtId="165" formatCode="0.00000000E+00"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -66,7 +78,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -75,6 +87,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -84,6 +97,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -132,7 +148,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -167,7 +183,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -728,10 +744,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K16"/>
+  <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1020,6 +1036,94 @@
         <v>1.9377559595290599E+19</v>
       </c>
     </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>6736</v>
+      </c>
+      <c r="B21" s="6">
+        <v>2.1802E+19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>2771</v>
+      </c>
+      <c r="B22" s="6">
+        <v>2.21423E+19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>9393</v>
+      </c>
+      <c r="B23" s="6">
+        <v>2.24469E+19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>4278</v>
+      </c>
+      <c r="B24" s="6">
+        <v>2.28697E+19</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>6494</v>
+      </c>
+      <c r="B25" s="6">
+        <v>2.30881E+19</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>9560</v>
+      </c>
+      <c r="B26" s="6">
+        <v>2.34592E+19</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>8839</v>
+      </c>
+      <c r="B27" s="6">
+        <v>2.36409E+19</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>2262</v>
+      </c>
+      <c r="B28" s="6">
+        <v>2.43383E+19</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>5411</v>
+      </c>
+      <c r="B29" s="6">
+        <v>2.43517E+19</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>4373</v>
+      </c>
+      <c r="B30" s="6">
+        <v>2.43994E+19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>